<commit_message>
suresh has made little changes
</commit_message>
<xml_diff>
--- a/src/test/java/com/mercurytours/properties/TestData.xlsx
+++ b/src/test/java/com/mercurytours/properties/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -26,12 +26,6 @@
   </si>
   <si>
     <t>suresh</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
 </sst>
 </file>
@@ -380,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,33 +396,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>